<commit_message>
implement ui and warm start with rl; start test agent.py
</commit_message>
<xml_diff>
--- a/data/nurse_preferences.xlsx
+++ b/data/nurse_preferences.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ishla\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D243975A-CBAB-48D7-A056-987C99F32173}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CDAC1A2-5687-4AE8-A339-3124AA282E8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{FDC03BBC-14F0-4933-B53B-6C77B02101BD}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="60">
   <si>
     <t>Thurs 2025-05-15</t>
   </si>
@@ -258,7 +258,18 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -570,8 +581,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{177EFD1A-DAA9-4EC3-8622-DB4ECE4F9DFE}">
   <dimension ref="A1:O43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="72" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+    <sheetView tabSelected="1" zoomScale="54" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -656,45 +667,41 @@
         <v>49</v>
       </c>
       <c r="C3"/>
-      <c r="D3"/>
+      <c r="D3" t="s">
+        <v>49</v>
+      </c>
       <c r="E3"/>
-      <c r="F3" t="s">
-        <v>49</v>
-      </c>
+      <c r="F3"/>
       <c r="G3"/>
-      <c r="H3"/>
+      <c r="H3" t="s">
+        <v>50</v>
+      </c>
       <c r="I3"/>
-      <c r="J3" t="s">
-        <v>49</v>
-      </c>
+      <c r="J3"/>
       <c r="K3"/>
       <c r="L3"/>
-      <c r="M3"/>
+      <c r="M3" t="s">
+        <v>48</v>
+      </c>
       <c r="N3"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B4"/>
-      <c r="C4" t="s">
-        <v>48</v>
-      </c>
+      <c r="B4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C4"/>
       <c r="D4"/>
       <c r="E4"/>
       <c r="F4"/>
-      <c r="G4" t="s">
-        <v>48</v>
-      </c>
-      <c r="H4" t="s">
-        <v>50</v>
-      </c>
+      <c r="G4"/>
+      <c r="H4"/>
       <c r="I4"/>
       <c r="J4"/>
       <c r="K4"/>
-      <c r="L4" t="s">
-        <v>49</v>
-      </c>
+      <c r="L4"/>
       <c r="M4"/>
       <c r="N4"/>
     </row>
@@ -702,7 +709,9 @@
       <c r="A5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B5"/>
+      <c r="B5" t="s">
+        <v>49</v>
+      </c>
       <c r="C5"/>
       <c r="D5"/>
       <c r="E5"/>
@@ -719,7 +728,9 @@
       <c r="A6" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B6"/>
+      <c r="B6" t="s">
+        <v>49</v>
+      </c>
       <c r="C6"/>
       <c r="D6"/>
       <c r="E6"/>
@@ -729,36 +740,73 @@
       <c r="I6"/>
       <c r="J6"/>
       <c r="K6"/>
+      <c r="M6"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>18</v>
       </c>
+      <c r="B7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C7"/>
+      <c r="J7"/>
+      <c r="M7"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>19</v>
       </c>
+      <c r="B8" t="s">
+        <v>49</v>
+      </c>
+      <c r="C8"/>
+      <c r="J8"/>
+      <c r="M8"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>20</v>
       </c>
+      <c r="B9" t="s">
+        <v>49</v>
+      </c>
+      <c r="C9"/>
+      <c r="J9"/>
+      <c r="M9"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>21</v>
       </c>
+      <c r="B10" t="s">
+        <v>49</v>
+      </c>
+      <c r="C10"/>
+      <c r="J10"/>
+      <c r="M10"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>22</v>
       </c>
+      <c r="B11" t="s">
+        <v>49</v>
+      </c>
+      <c r="C11"/>
+      <c r="J11"/>
+      <c r="K11" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="M11"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>23</v>
       </c>
+      <c r="B12" t="s">
+        <v>49</v>
+      </c>
       <c r="F12" s="1" t="s">
         <v>58</v>
       </c>
@@ -768,6 +816,7 @@
       <c r="L12" s="1" t="s">
         <v>58</v>
       </c>
+      <c r="M12"/>
       <c r="N12" s="1" t="s">
         <v>58</v>
       </c>
@@ -776,96 +825,157 @@
       <c r="A13" s="1" t="s">
         <v>24</v>
       </c>
+      <c r="B13" t="s">
+        <v>49</v>
+      </c>
+      <c r="M13"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>25</v>
       </c>
+      <c r="B14" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>26</v>
       </c>
+      <c r="B15" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>27</v>
       </c>
+      <c r="B16" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>28</v>
       </c>
+      <c r="B17" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>29</v>
       </c>
+      <c r="B18" t="s">
+        <v>49</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>30</v>
       </c>
+      <c r="B19" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>31</v>
       </c>
+      <c r="B20" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>32</v>
       </c>
+      <c r="B21" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>33</v>
       </c>
+      <c r="B22" t="s">
+        <v>49</v>
+      </c>
       <c r="H22"/>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>51</v>
       </c>
+      <c r="B23" t="s">
+        <v>49</v>
+      </c>
       <c r="H23"/>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
         <v>55</v>
       </c>
+      <c r="B24" t="s">
+        <v>49</v>
+      </c>
       <c r="H24"/>
+      <c r="I24" s="1" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
         <v>56</v>
       </c>
+      <c r="B25" t="s">
+        <v>49</v>
+      </c>
       <c r="H25"/>
+      <c r="I25" s="1" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
         <v>57</v>
       </c>
+      <c r="B26" t="s">
+        <v>49</v>
+      </c>
       <c r="H26"/>
+      <c r="I26" s="1" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
         <v>34</v>
       </c>
+      <c r="B27" t="s">
+        <v>49</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B28"/>
-      <c r="C28"/>
+      <c r="B28" t="s">
+        <v>49</v>
+      </c>
       <c r="D28"/>
       <c r="E28"/>
       <c r="F28"/>
-      <c r="G28"/>
       <c r="H28"/>
-      <c r="I28"/>
-      <c r="J28"/>
-      <c r="K28"/>
+      <c r="I28" s="1" t="s">
+        <v>50</v>
+      </c>
       <c r="L28"/>
       <c r="M28"/>
       <c r="N28"/>
@@ -875,30 +985,26 @@
         <v>36</v>
       </c>
       <c r="B29"/>
-      <c r="C29"/>
       <c r="D29"/>
       <c r="E29"/>
       <c r="F29"/>
-      <c r="G29"/>
       <c r="H29"/>
-      <c r="I29"/>
-      <c r="J29"/>
-      <c r="K29"/>
+      <c r="I29" s="1" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
         <v>37</v>
       </c>
       <c r="B30"/>
-      <c r="C30"/>
       <c r="D30"/>
       <c r="E30"/>
       <c r="F30"/>
-      <c r="G30"/>
       <c r="H30"/>
-      <c r="I30"/>
-      <c r="J30"/>
-      <c r="K30"/>
+      <c r="I30" s="1" t="s">
+        <v>50</v>
+      </c>
       <c r="L30"/>
       <c r="M30"/>
     </row>
@@ -907,39 +1013,30 @@
         <v>38</v>
       </c>
       <c r="B31"/>
-      <c r="C31"/>
       <c r="D31"/>
-      <c r="E31" t="s">
-        <v>49</v>
-      </c>
+      <c r="E31"/>
       <c r="F31"/>
-      <c r="G31"/>
-      <c r="H31" t="s">
-        <v>49</v>
-      </c>
-      <c r="I31" t="s">
-        <v>49</v>
-      </c>
-      <c r="J31"/>
+      <c r="H31"/>
+      <c r="I31" s="1" t="s">
+        <v>50</v>
+      </c>
       <c r="K31"/>
       <c r="L31"/>
       <c r="M31"/>
-      <c r="N31" t="s">
-        <v>49</v>
-      </c>
+      <c r="N31"/>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
         <v>39</v>
       </c>
       <c r="B32"/>
-      <c r="C32"/>
       <c r="D32"/>
       <c r="E32"/>
       <c r="F32"/>
-      <c r="G32"/>
       <c r="H32"/>
-      <c r="J32"/>
+      <c r="I32" s="1" t="s">
+        <v>50</v>
+      </c>
       <c r="K32"/>
       <c r="L32"/>
     </row>
@@ -947,17 +1044,23 @@
       <c r="A33" s="1" t="s">
         <v>40</v>
       </c>
+      <c r="I33" s="1" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
         <v>41</v>
       </c>
+      <c r="I34" s="1" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="I35" s="1" t="s">
         <v>50</v>
       </c>
     </row>
@@ -965,26 +1068,53 @@
       <c r="A36" s="1" t="s">
         <v>43</v>
       </c>
+      <c r="B36" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="I36" s="1" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
         <v>44</v>
       </c>
+      <c r="B37" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="I37" s="1" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
         <v>45</v>
       </c>
+      <c r="B38" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="I38" s="1" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
         <v>46</v>
       </c>
+      <c r="B39" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="I39" s="1" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
         <v>47</v>
       </c>
+      <c r="B40" s="1" t="s">
+        <v>48</v>
+      </c>
       <c r="N40" s="1" t="s">
         <v>58</v>
       </c>
@@ -996,19 +1126,33 @@
       <c r="A41" s="1" t="s">
         <v>52</v>
       </c>
+      <c r="B41" s="1" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
         <v>53</v>
       </c>
+      <c r="B42" s="1" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
         <v>54</v>
       </c>
+      <c r="B43" s="1" t="s">
+        <v>48</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
+  <conditionalFormatting sqref="A1:XFD1048576">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+      <formula>"MC"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
set parameters; model for 7, 14, 28 days; start work on EL
</commit_message>
<xml_diff>
--- a/data/nurse_preferences.xlsx
+++ b/data/nurse_preferences.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ishla\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CDAC1A2-5687-4AE8-A339-3124AA282E8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8080C36B-D3A4-4EE0-8CB1-BF8ED761C7C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{FDC03BBC-14F0-4933-B53B-6C77B02101BD}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="74">
   <si>
     <t>Thurs 2025-05-15</t>
   </si>
@@ -205,6 +205,48 @@
   </si>
   <si>
     <t>Wed 2025-05-28</t>
+  </si>
+  <si>
+    <t>Thurs 2025-05-29</t>
+  </si>
+  <si>
+    <t>Fri 2025-05-30</t>
+  </si>
+  <si>
+    <t>Sat 2025-05-31</t>
+  </si>
+  <si>
+    <t>Sun 2025-06-01</t>
+  </si>
+  <si>
+    <t>Mon 2025-06-02</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Tues 2025-06-03</t>
+  </si>
+  <si>
+    <t>Wed 2025-06-04</t>
+  </si>
+  <si>
+    <t>Thurs 2025-06-05</t>
+  </si>
+  <si>
+    <t>Fri 2025-06-06</t>
+  </si>
+  <si>
+    <t>Sat 2025-06-07</t>
+  </si>
+  <si>
+    <t>Sun 2025-06-08</t>
+  </si>
+  <si>
+    <t>Mon 2025-06-09</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Tues 2025-06-10</t>
+  </si>
+  <si>
+    <t>Wed 2025-06-11</t>
   </si>
 </sst>
 </file>
@@ -246,13 +288,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -579,21 +624,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{177EFD1A-DAA9-4EC3-8622-DB4ECE4F9DFE}">
-  <dimension ref="A1:O43"/>
+  <dimension ref="A1:AC43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="54" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="8.7265625" style="1"/>
-    <col min="2" max="14" width="15.453125" style="1" customWidth="1"/>
-    <col min="15" max="15" width="15.1796875" style="1" customWidth="1"/>
-    <col min="16" max="16384" width="8.7265625" style="1"/>
+    <col min="2" max="15" width="16.08984375" style="1" customWidth="1"/>
+    <col min="16" max="29" width="15.453125" style="1" customWidth="1"/>
+    <col min="30" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:29" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
@@ -636,175 +681,217 @@
       <c r="O1" s="2" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P1" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="V1" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="W1" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="X1" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y1" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="Z1" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="AA1" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="AB1" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="AC1" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="C2"/>
-      <c r="D2"/>
-      <c r="E2" t="s">
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="F2"/>
-      <c r="G2"/>
-      <c r="H2"/>
-      <c r="I2"/>
-      <c r="J2"/>
-      <c r="K2"/>
-      <c r="L2"/>
-      <c r="M2"/>
-      <c r="N2"/>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+    </row>
+    <row r="3" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B3" t="s">
-        <v>49</v>
-      </c>
-      <c r="C3"/>
-      <c r="D3" t="s">
-        <v>49</v>
-      </c>
-      <c r="E3"/>
-      <c r="F3"/>
-      <c r="G3"/>
-      <c r="H3" t="s">
-        <v>50</v>
-      </c>
-      <c r="I3"/>
-      <c r="J3"/>
-      <c r="K3"/>
-      <c r="L3"/>
-      <c r="M3" t="s">
+      <c r="B3" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="N3"/>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="N3" s="3"/>
+    </row>
+    <row r="4" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B4" t="s">
-        <v>49</v>
-      </c>
-      <c r="C4"/>
-      <c r="D4"/>
-      <c r="E4"/>
-      <c r="F4"/>
-      <c r="G4"/>
-      <c r="H4"/>
-      <c r="I4"/>
-      <c r="J4"/>
-      <c r="K4"/>
-      <c r="L4"/>
-      <c r="M4"/>
-      <c r="N4"/>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="B4" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
+    </row>
+    <row r="5" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B5" t="s">
-        <v>49</v>
-      </c>
-      <c r="C5"/>
-      <c r="D5"/>
-      <c r="E5"/>
-      <c r="F5"/>
-      <c r="G5"/>
-      <c r="H5"/>
-      <c r="I5"/>
-      <c r="J5"/>
-      <c r="K5"/>
-      <c r="L5"/>
-      <c r="M5"/>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="B5" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
+    </row>
+    <row r="6" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B6" t="s">
-        <v>49</v>
-      </c>
-      <c r="C6"/>
-      <c r="D6"/>
-      <c r="E6"/>
-      <c r="F6"/>
-      <c r="G6"/>
-      <c r="H6"/>
-      <c r="I6"/>
-      <c r="J6"/>
-      <c r="K6"/>
-      <c r="M6"/>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="B6" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="M6" s="3"/>
+    </row>
+    <row r="7" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B7" t="s">
-        <v>49</v>
-      </c>
-      <c r="C7"/>
-      <c r="J7"/>
-      <c r="M7"/>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="B7" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="M7" s="3"/>
+    </row>
+    <row r="8" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B8" t="s">
-        <v>49</v>
-      </c>
-      <c r="C8"/>
-      <c r="J8"/>
-      <c r="M8"/>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="B8" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="M8" s="3"/>
+    </row>
+    <row r="9" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B9" t="s">
-        <v>49</v>
-      </c>
-      <c r="C9"/>
-      <c r="J9"/>
-      <c r="M9"/>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="B9" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C9" s="3"/>
+      <c r="J9" s="3"/>
+      <c r="M9" s="3"/>
+    </row>
+    <row r="10" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B10" t="s">
-        <v>49</v>
-      </c>
-      <c r="C10"/>
-      <c r="J10"/>
-      <c r="M10"/>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="B10" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C10" s="3"/>
+      <c r="J10" s="3"/>
+      <c r="M10" s="3"/>
+    </row>
+    <row r="11" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B11" t="s">
-        <v>49</v>
-      </c>
-      <c r="C11"/>
-      <c r="J11"/>
+      <c r="B11" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C11" s="3"/>
+      <c r="J11" s="3"/>
       <c r="K11" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="M11"/>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="M11" s="3"/>
+    </row>
+    <row r="12" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="3" t="s">
         <v>49</v>
       </c>
       <c r="F12" s="1" t="s">
@@ -816,41 +903,44 @@
       <c r="L12" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="M12"/>
+      <c r="M12" s="3"/>
       <c r="N12" s="1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B13" t="s">
-        <v>49</v>
-      </c>
-      <c r="M13"/>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="B13" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="M13" s="3"/>
+    </row>
+    <row r="14" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B14" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="B14" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="15" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B15" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="B15" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="V15" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="16" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="3" t="s">
         <v>49</v>
       </c>
     </row>
@@ -858,7 +948,7 @@
       <c r="A17" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="3" t="s">
         <v>49</v>
       </c>
     </row>
@@ -866,7 +956,7 @@
       <c r="A18" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="3" t="s">
         <v>49</v>
       </c>
       <c r="E18" s="1" t="s">
@@ -877,7 +967,7 @@
       <c r="A19" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="3" t="s">
         <v>49</v>
       </c>
     </row>
@@ -885,7 +975,7 @@
       <c r="A20" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="3" t="s">
         <v>49</v>
       </c>
     </row>
@@ -893,7 +983,7 @@
       <c r="A21" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="3" t="s">
         <v>49</v>
       </c>
     </row>
@@ -901,28 +991,28 @@
       <c r="A22" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B22" t="s">
-        <v>49</v>
-      </c>
-      <c r="H22"/>
+      <c r="B22" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H22" s="3"/>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B23" t="s">
-        <v>49</v>
-      </c>
-      <c r="H23"/>
+      <c r="B23" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H23" s="3"/>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B24" t="s">
-        <v>49</v>
-      </c>
-      <c r="H24"/>
+      <c r="B24" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H24" s="3"/>
       <c r="I24" s="1" t="s">
         <v>50</v>
       </c>
@@ -931,10 +1021,10 @@
       <c r="A25" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B25" t="s">
-        <v>49</v>
-      </c>
-      <c r="H25"/>
+      <c r="B25" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H25" s="3"/>
       <c r="I25" s="1" t="s">
         <v>50</v>
       </c>
@@ -943,10 +1033,10 @@
       <c r="A26" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B26" t="s">
-        <v>49</v>
-      </c>
-      <c r="H26"/>
+      <c r="B26" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H26" s="3"/>
       <c r="I26" s="1" t="s">
         <v>50</v>
       </c>
@@ -955,7 +1045,7 @@
       <c r="A27" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="3" t="s">
         <v>49</v>
       </c>
       <c r="I27" s="1" t="s">
@@ -966,29 +1056,29 @@
       <c r="A28" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B28" t="s">
-        <v>49</v>
-      </c>
-      <c r="D28"/>
-      <c r="E28"/>
-      <c r="F28"/>
-      <c r="H28"/>
+      <c r="B28" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3"/>
+      <c r="H28" s="3"/>
       <c r="I28" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="L28"/>
-      <c r="M28"/>
-      <c r="N28"/>
+      <c r="L28" s="3"/>
+      <c r="M28" s="3"/>
+      <c r="N28" s="3"/>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B29"/>
-      <c r="D29"/>
-      <c r="E29"/>
-      <c r="F29"/>
-      <c r="H29"/>
+      <c r="B29" s="3"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="3"/>
+      <c r="H29" s="3"/>
       <c r="I29" s="1" t="s">
         <v>50</v>
       </c>
@@ -997,48 +1087,48 @@
       <c r="A30" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B30"/>
-      <c r="D30"/>
-      <c r="E30"/>
-      <c r="F30"/>
-      <c r="H30"/>
+      <c r="B30" s="3"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="3"/>
+      <c r="H30" s="3"/>
       <c r="I30" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="L30"/>
-      <c r="M30"/>
+      <c r="L30" s="3"/>
+      <c r="M30" s="3"/>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B31"/>
-      <c r="D31"/>
-      <c r="E31"/>
-      <c r="F31"/>
-      <c r="H31"/>
+      <c r="B31" s="3"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="3"/>
+      <c r="H31" s="3"/>
       <c r="I31" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="K31"/>
-      <c r="L31"/>
-      <c r="M31"/>
-      <c r="N31"/>
+      <c r="K31" s="3"/>
+      <c r="L31" s="3"/>
+      <c r="M31" s="3"/>
+      <c r="N31" s="3"/>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B32"/>
-      <c r="D32"/>
-      <c r="E32"/>
-      <c r="F32"/>
-      <c r="H32"/>
+      <c r="B32" s="3"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
+      <c r="F32" s="3"/>
+      <c r="H32" s="3"/>
       <c r="I32" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="K32"/>
-      <c r="L32"/>
+      <c r="K32" s="3"/>
+      <c r="L32" s="3"/>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
@@ -1141,9 +1231,6 @@
     <row r="43" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
         <v>54</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>